<commit_message>
Completed Feature ID: GUI. Still need to implement and complete Feature ID: IGUI.
</commit_message>
<xml_diff>
--- a/P06/Scrum.xlsx
+++ b/P06/Scrum.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="192">
   <si>
     <t xml:space="preserve">Product Name:</t>
   </si>
@@ -172,6 +172,9 @@
     <t xml:space="preserve">GUI</t>
   </si>
   <si>
+    <t xml:space="preserve">Finished in Sprint 2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Use a GUI instead of a terminal</t>
   </si>
   <si>
@@ -182,6 +185,9 @@
   </si>
   <si>
     <t xml:space="preserve">IGUI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In Work</t>
   </si>
   <si>
     <t xml:space="preserve">Use dialogs to create items</t>
@@ -595,13 +601,16 @@
     <t xml:space="preserve">MixIn Class created. Debugging toString Method for multiple MixIns.</t>
   </si>
   <si>
-    <t xml:space="preserve">In Work</t>
-  </si>
-  <si>
     <t xml:space="preserve">Scoop Class created. Debugging toString Method for multiple MixIns.</t>
   </si>
   <si>
     <t xml:space="preserve">Fixed toString method in Scoop to print multiple toppings.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Created a GUI instead of a Terminal, with all MenuItems created</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Need to implement ActionListeners for each MenuItem.</t>
   </si>
   <si>
     <t xml:space="preserve">--&gt; Add tasks to complete each feature for this sprint</t>
@@ -1140,10 +1149,10 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1158,11 +1167,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="39115637"/>
-        <c:axId val="65821550"/>
+        <c:axId val="51850467"/>
+        <c:axId val="23113389"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="39115637"/>
+        <c:axId val="51850467"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1227,7 +1236,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65821550"/>
+        <c:crossAx val="23113389"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1235,7 +1244,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="65821550"/>
+        <c:axId val="23113389"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1309,7 +1318,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="39115637"/>
+        <c:crossAx val="51850467"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1329,7 +1338,7 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
@@ -1464,11 +1473,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="58082711"/>
-        <c:axId val="77267579"/>
+        <c:axId val="35968252"/>
+        <c:axId val="30133658"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="58082711"/>
+        <c:axId val="35968252"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1533,7 +1542,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77267579"/>
+        <c:crossAx val="30133658"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1541,7 +1550,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="77267579"/>
+        <c:axId val="30133658"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1615,7 +1624,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="58082711"/>
+        <c:crossAx val="35968252"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1635,7 +1644,7 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
@@ -1770,11 +1779,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="37687842"/>
-        <c:axId val="74731961"/>
+        <c:axId val="90605911"/>
+        <c:axId val="88890825"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="37687842"/>
+        <c:axId val="90605911"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1839,7 +1848,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74731961"/>
+        <c:crossAx val="88890825"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1847,7 +1856,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="74731961"/>
+        <c:axId val="88890825"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1921,7 +1930,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="37687842"/>
+        <c:crossAx val="90605911"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1941,7 +1950,7 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
@@ -2076,11 +2085,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="61307439"/>
-        <c:axId val="14725570"/>
+        <c:axId val="30058506"/>
+        <c:axId val="36244297"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="61307439"/>
+        <c:axId val="30058506"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2145,7 +2154,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="14725570"/>
+        <c:crossAx val="36244297"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2153,7 +2162,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="14725570"/>
+        <c:axId val="36244297"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2227,7 +2236,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61307439"/>
+        <c:crossAx val="30058506"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2247,7 +2256,7 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
@@ -2382,11 +2391,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="57320933"/>
-        <c:axId val="55599664"/>
+        <c:axId val="13294067"/>
+        <c:axId val="74452125"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="57320933"/>
+        <c:axId val="13294067"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2451,7 +2460,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="55599664"/>
+        <c:crossAx val="74452125"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2459,7 +2468,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="55599664"/>
+        <c:axId val="74452125"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2533,7 +2542,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="57320933"/>
+        <c:crossAx val="13294067"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2553,7 +2562,7 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
@@ -2606,10 +2615,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0822405395279131"/>
-          <c:y val="0.161875945537065"/>
-          <c:w val="0.884351192706382"/>
-          <c:h val="0.63565305093293"/>
+          <c:x val="0.0822456753887466"/>
+          <c:y val="0.161896356071113"/>
+          <c:w val="0.884281521263973"/>
+          <c:h val="0.635607111335267"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -2699,30 +2708,30 @@
                   <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>36</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>36</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>36</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>36</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>36</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="55762341"/>
-        <c:axId val="96862703"/>
+        <c:axId val="93107994"/>
+        <c:axId val="93517615"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="55762341"/>
+        <c:axId val="93107994"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -2789,12 +2798,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="96862703"/>
+        <c:crossAx val="93517615"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="96862703"/>
+        <c:axId val="93517615"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -2869,7 +2878,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="55762341"/>
+        <c:crossAx val="93107994"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2889,7 +2898,7 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
@@ -3024,11 +3033,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="85331180"/>
-        <c:axId val="43457400"/>
+        <c:axId val="85731845"/>
+        <c:axId val="63902455"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="85331180"/>
+        <c:axId val="85731845"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3093,7 +3102,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43457400"/>
+        <c:crossAx val="63902455"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3101,7 +3110,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="43457400"/>
+        <c:axId val="63902455"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3175,7 +3184,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85331180"/>
+        <c:crossAx val="85731845"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3195,7 +3204,7 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
@@ -3213,9 +3222,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>3202200</xdr:colOff>
+      <xdr:colOff>3201840</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>120600</xdr:rowOff>
+      <xdr:rowOff>120240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3223,8 +3232,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9118080" y="268200"/>
-        <a:ext cx="5764680" cy="2855160"/>
+        <a:off x="9116280" y="268200"/>
+        <a:ext cx="5764320" cy="2854800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3248,9 +3257,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>518400</xdr:colOff>
+      <xdr:colOff>518040</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>129600</xdr:rowOff>
+      <xdr:rowOff>129240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3258,8 +3267,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4088880" y="446400"/>
-        <a:ext cx="3747240" cy="1847880"/>
+        <a:off x="4090680" y="446400"/>
+        <a:ext cx="3747600" cy="1847520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3283,9 +3292,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>518400</xdr:colOff>
+      <xdr:colOff>518040</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>129600</xdr:rowOff>
+      <xdr:rowOff>129240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3293,8 +3302,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4088880" y="446400"/>
-        <a:ext cx="3747240" cy="1847880"/>
+        <a:off x="4090680" y="446400"/>
+        <a:ext cx="3747600" cy="1847520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3318,9 +3327,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>518400</xdr:colOff>
+      <xdr:colOff>518040</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>129600</xdr:rowOff>
+      <xdr:rowOff>129240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3328,8 +3337,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4088880" y="446400"/>
-        <a:ext cx="3747240" cy="1847880"/>
+        <a:off x="4090680" y="446400"/>
+        <a:ext cx="3747600" cy="1847520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3353,9 +3362,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>518400</xdr:colOff>
+      <xdr:colOff>518040</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>129600</xdr:rowOff>
+      <xdr:rowOff>129240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3363,8 +3372,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4088880" y="446400"/>
-        <a:ext cx="3747240" cy="1847880"/>
+        <a:off x="4090680" y="446400"/>
+        <a:ext cx="3747600" cy="1847520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3388,9 +3397,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>518400</xdr:colOff>
+      <xdr:colOff>518040</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>129600</xdr:rowOff>
+      <xdr:rowOff>129240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3398,8 +3407,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4088880" y="446400"/>
-        <a:ext cx="3747240" cy="1847880"/>
+        <a:off x="4090680" y="446400"/>
+        <a:ext cx="3747600" cy="1847520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3423,9 +3432,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>518400</xdr:colOff>
+      <xdr:colOff>518040</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>129600</xdr:rowOff>
+      <xdr:rowOff>129240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3433,8 +3442,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4088880" y="446400"/>
-        <a:ext cx="3747240" cy="1847880"/>
+        <a:off x="4090680" y="446400"/>
+        <a:ext cx="3747600" cy="1847520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3455,8 +3464,8 @@
   </sheetPr>
   <dimension ref="A1:K102"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G31" activeCellId="0" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3464,11 +3473,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="4.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="8.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="8.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="17.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="9.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="9.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="45.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="39.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="53.71"/>
@@ -3636,11 +3645,11 @@
       </c>
       <c r="B14" s="3" t="n">
         <f aca="false">B13-C14</f>
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C14" s="10" t="n">
         <f aca="false">COUNTIF(G$24:G$108,"Finished in Sprint 2")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="3"/>
@@ -3660,7 +3669,7 @@
       </c>
       <c r="B15" s="3" t="n">
         <f aca="false">B14-C15</f>
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C15" s="10" t="n">
         <f aca="false">COUNTIF(G$24:G$108,"Finished in Sprint 3")</f>
@@ -3684,7 +3693,7 @@
       </c>
       <c r="B16" s="3" t="n">
         <f aca="false">B15-C16</f>
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C16" s="10" t="n">
         <f aca="false">COUNTIF(G$24:G$108,"Finished in Sprint 4")</f>
@@ -3704,7 +3713,7 @@
       </c>
       <c r="B17" s="3" t="n">
         <f aca="false">B16-C17</f>
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C17" s="10" t="n">
         <f aca="false">COUNTIF(G$24:G$108,"Finished in Sprint 5")</f>
@@ -3724,7 +3733,7 @@
       </c>
       <c r="B18" s="3" t="n">
         <f aca="false">B17-C18</f>
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C18" s="10" t="n">
         <f aca="false">COUNTIF(G$24:G$108,"Finished in Sprint 6")</f>
@@ -3976,23 +3985,25 @@
       <c r="F28" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="G28" s="18"/>
+      <c r="G28" s="18" t="s">
+        <v>48</v>
+      </c>
       <c r="H28" s="14" t="s">
         <v>32</v>
       </c>
       <c r="I28" s="19" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J28" s="19" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K28" s="19" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B29" s="11" t="n">
         <v>6</v>
@@ -4007,23 +4018,25 @@
       <c r="F29" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="G29" s="18"/>
+      <c r="G29" s="18" t="s">
+        <v>53</v>
+      </c>
       <c r="H29" s="14" t="s">
         <v>32</v>
       </c>
       <c r="I29" s="19" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="J29" s="19" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K29" s="19" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B30" s="11" t="n">
         <v>7</v>
@@ -4038,21 +4051,21 @@
       <c r="F30" s="17"/>
       <c r="G30" s="18"/>
       <c r="H30" s="14" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I30" s="19" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="J30" s="19" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K30" s="19" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B31" s="11" t="n">
         <v>8</v>
@@ -4070,18 +4083,18 @@
         <v>32</v>
       </c>
       <c r="I31" s="19" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="J31" s="19" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K31" s="19" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="32" s="20" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B32" s="11" t="n">
         <v>9</v>
@@ -4099,16 +4112,16 @@
         <v>32</v>
       </c>
       <c r="I32" s="19" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J32" s="19" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="K32" s="19"/>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B33" s="11" t="n">
         <v>10</v>
@@ -4123,19 +4136,19 @@
       <c r="F33" s="17"/>
       <c r="G33" s="18"/>
       <c r="H33" s="14" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I33" s="19" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="J33" s="19" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="K33" s="19"/>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B34" s="11" t="n">
         <v>11</v>
@@ -4150,19 +4163,19 @@
       <c r="F34" s="17"/>
       <c r="G34" s="18"/>
       <c r="H34" s="14" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I34" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="J34" s="19" t="s">
         <v>70</v>
-      </c>
-      <c r="J34" s="19" t="s">
-        <v>68</v>
       </c>
       <c r="K34" s="19"/>
     </row>
     <row r="35" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B35" s="11" t="n">
         <v>12</v>
@@ -4180,18 +4193,18 @@
         <v>32</v>
       </c>
       <c r="I35" s="19" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="J35" s="19" t="s">
         <v>34</v>
       </c>
       <c r="K35" s="19" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B36" s="11" t="n">
         <v>13</v>
@@ -4206,21 +4219,21 @@
       <c r="F36" s="17"/>
       <c r="G36" s="18"/>
       <c r="H36" s="14" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="I36" s="19" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J36" s="19" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="K36" s="19" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="37" s="20" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B37" s="11" t="n">
         <v>14</v>
@@ -4238,16 +4251,16 @@
         <v>32</v>
       </c>
       <c r="I37" s="19" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="J37" s="19" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="K37" s="19"/>
     </row>
     <row r="38" s="20" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B38" s="11" t="n">
         <v>15</v>
@@ -4262,19 +4275,19 @@
       <c r="F38" s="17"/>
       <c r="G38" s="18"/>
       <c r="H38" s="14" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="I38" s="19" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J38" s="19" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="K38" s="19"/>
     </row>
     <row r="39" s="20" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B39" s="11" t="n">
         <v>16</v>
@@ -4289,19 +4302,19 @@
       <c r="F39" s="17"/>
       <c r="G39" s="18"/>
       <c r="H39" s="14" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="I39" s="19" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="J39" s="19" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="K39" s="19"/>
     </row>
     <row r="40" s="20" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B40" s="11" t="n">
         <v>17</v>
@@ -4316,21 +4329,21 @@
       <c r="F40" s="17"/>
       <c r="G40" s="18"/>
       <c r="H40" s="14" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I40" s="19" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="J40" s="19" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="K40" s="19" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="41" s="20" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B41" s="11" t="n">
         <v>18</v>
@@ -4345,21 +4358,21 @@
       <c r="F41" s="17"/>
       <c r="G41" s="18"/>
       <c r="H41" s="14" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I41" s="19" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="J41" s="19" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="K41" s="19" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="42" s="20" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B42" s="11" t="n">
         <v>19</v>
@@ -4377,18 +4390,18 @@
         <v>32</v>
       </c>
       <c r="I42" s="19" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="J42" s="19" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="K42" s="19" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="43" s="20" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B43" s="11" t="n">
         <v>20</v>
@@ -4406,16 +4419,16 @@
         <v>32</v>
       </c>
       <c r="I43" s="19" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="J43" s="19" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="K43" s="19"/>
     </row>
     <row r="44" s="20" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B44" s="11" t="n">
         <v>21</v>
@@ -4430,21 +4443,21 @@
       <c r="F44" s="17"/>
       <c r="G44" s="18"/>
       <c r="H44" s="14" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="I44" s="19" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="J44" s="19" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="K44" s="19" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="45" s="20" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B45" s="11" t="n">
         <v>22</v>
@@ -4459,21 +4472,21 @@
       <c r="F45" s="17"/>
       <c r="G45" s="18"/>
       <c r="H45" s="14" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I45" s="19" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="J45" s="19" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="K45" s="19" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B46" s="11" t="n">
         <v>23</v>
@@ -4488,21 +4501,21 @@
       <c r="F46" s="17"/>
       <c r="G46" s="18"/>
       <c r="H46" s="14" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I46" s="19" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="J46" s="19" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="K46" s="19" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B47" s="11" t="n">
         <v>24</v>
@@ -4515,19 +4528,19 @@
       <c r="F47" s="17"/>
       <c r="G47" s="18"/>
       <c r="H47" s="14" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I47" s="19" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="J47" s="19" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="K47" s="19"/>
     </row>
     <row r="48" s="20" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B48" s="11" t="n">
         <v>25</v>
@@ -4540,19 +4553,19 @@
       <c r="F48" s="17"/>
       <c r="G48" s="18"/>
       <c r="H48" s="14" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I48" s="19" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="J48" s="19" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="K48" s="19"/>
     </row>
     <row r="49" s="21" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B49" s="11" t="n">
         <v>26</v>
@@ -4568,16 +4581,16 @@
         <v>32</v>
       </c>
       <c r="I49" s="19" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="J49" s="19" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="K49" s="19"/>
     </row>
     <row r="50" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B50" s="11" t="n">
         <v>27</v>
@@ -4593,16 +4606,16 @@
         <v>32</v>
       </c>
       <c r="I50" s="19" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="J50" s="19" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="K50" s="19"/>
     </row>
     <row r="51" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B51" s="11" t="n">
         <v>28</v>
@@ -4618,16 +4631,16 @@
         <v>32</v>
       </c>
       <c r="I51" s="19" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="J51" s="19" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="K51" s="19"/>
     </row>
     <row r="52" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B52" s="11" t="n">
         <v>29</v>
@@ -4643,16 +4656,16 @@
         <v>32</v>
       </c>
       <c r="I52" s="19" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="J52" s="19" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="K52" s="19"/>
     </row>
     <row r="53" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B53" s="11" t="n">
         <v>30</v>
@@ -4665,19 +4678,19 @@
       <c r="F53" s="17"/>
       <c r="G53" s="18"/>
       <c r="H53" s="14" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="I53" s="19" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="J53" s="19" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="K53" s="19"/>
     </row>
     <row r="54" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B54" s="11" t="n">
         <v>31</v>
@@ -4690,21 +4703,21 @@
       <c r="F54" s="17"/>
       <c r="G54" s="18"/>
       <c r="H54" s="14" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I54" s="19" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="J54" s="19" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="K54" s="19" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B55" s="11" t="n">
         <v>32</v>
@@ -4720,16 +4733,16 @@
         <v>32</v>
       </c>
       <c r="I55" s="19" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="J55" s="19" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="K55" s="19"/>
     </row>
     <row r="56" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B56" s="11" t="n">
         <v>33</v>
@@ -4745,16 +4758,16 @@
         <v>32</v>
       </c>
       <c r="I56" s="19" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="J56" s="19" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="K56" s="19"/>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B57" s="11" t="n">
         <v>34</v>
@@ -4770,16 +4783,16 @@
         <v>32</v>
       </c>
       <c r="I57" s="19" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="J57" s="19" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="K57" s="19"/>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B58" s="11" t="n">
         <v>35</v>
@@ -4795,16 +4808,16 @@
         <v>32</v>
       </c>
       <c r="I58" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="J58" s="19" t="s">
         <v>147</v>
-      </c>
-      <c r="J58" s="19" t="s">
-        <v>145</v>
       </c>
       <c r="K58" s="19"/>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B59" s="11" t="n">
         <v>36</v>
@@ -4820,16 +4833,16 @@
         <v>32</v>
       </c>
       <c r="I59" s="19" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="J59" s="19" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="K59" s="19"/>
     </row>
     <row r="60" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B60" s="11" t="n">
         <v>37</v>
@@ -4845,16 +4858,16 @@
         <v>32</v>
       </c>
       <c r="I60" s="19" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="J60" s="19" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="K60" s="19"/>
     </row>
     <row r="61" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B61" s="11" t="n">
         <v>38</v>
@@ -4870,16 +4883,16 @@
         <v>32</v>
       </c>
       <c r="I61" s="19" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="J61" s="19" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="K61" s="19"/>
     </row>
     <row r="62" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B62" s="11" t="n">
         <v>39</v>
@@ -4895,16 +4908,16 @@
         <v>32</v>
       </c>
       <c r="I62" s="19" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="J62" s="19" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="K62" s="19"/>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B63" s="11" t="n">
         <v>40</v>
@@ -4920,10 +4933,10 @@
         <v>32</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="J63" s="19" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="K63" s="19"/>
     </row>
@@ -5427,7 +5440,7 @@
       <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -5451,21 +5464,21 @@
     </row>
     <row r="2" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B2" s="25" t="n">
         <v>44831</v>
       </c>
       <c r="C2" s="22"/>
       <c r="D2" s="26" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="22"/>
     </row>
     <row r="3" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B3" s="25" t="n">
         <v>44838</v>
@@ -5477,10 +5490,10 @@
     </row>
     <row r="4" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="22" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C4" s="22"/>
       <c r="D4" s="22"/>
@@ -5501,7 +5514,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
@@ -5509,7 +5522,7 @@
     </row>
     <row r="7" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="22" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B7" s="22" t="n">
         <v>4</v>
@@ -5521,7 +5534,7 @@
     </row>
     <row r="8" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="22" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B8" s="22" t="n">
         <f aca="false">B7-C8</f>
@@ -5537,7 +5550,7 @@
     </row>
     <row r="9" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="22" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B9" s="22" t="n">
         <f aca="false">B8-C9</f>
@@ -5553,7 +5566,7 @@
     </row>
     <row r="10" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="22" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B10" s="22" t="n">
         <f aca="false">B9-C10</f>
@@ -5569,7 +5582,7 @@
     </row>
     <row r="11" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="22" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B11" s="22" t="n">
         <f aca="false">B10-C11</f>
@@ -5585,7 +5598,7 @@
     </row>
     <row r="12" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="22" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B12" s="22" t="n">
         <f aca="false">B11-C12</f>
@@ -5601,7 +5614,7 @@
     </row>
     <row r="13" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="22" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B13" s="22" t="n">
         <f aca="false">B12-C13</f>
@@ -5617,7 +5630,7 @@
     </row>
     <row r="14" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="22" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B14" s="22" t="n">
         <f aca="false">B13-C14</f>
@@ -5641,16 +5654,16 @@
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="29" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B16" s="29" t="s">
         <v>20</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E16" s="29" t="s">
         <v>25</v>
@@ -5667,10 +5680,10 @@
         <v>30</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5681,10 +5694,10 @@
         <v>36</v>
       </c>
       <c r="D18" s="30" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5695,10 +5708,10 @@
         <v>39</v>
       </c>
       <c r="D19" s="30" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="E19" s="32" t="s">
-        <v>183</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5709,10 +5722,10 @@
         <v>43</v>
       </c>
       <c r="D20" s="30" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E20" s="32" t="s">
-        <v>183</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5723,10 +5736,10 @@
         <v>39</v>
       </c>
       <c r="D21" s="30" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E21" s="32" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5737,10 +5750,10 @@
         <v>43</v>
       </c>
       <c r="D22" s="30" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E22" s="32" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6416,11 +6429,11 @@
   </sheetPr>
   <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -6445,7 +6458,7 @@
     </row>
     <row r="2" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B2" s="25" t="n">
         <f aca="false">'Sprint 01 Backlog'!B3</f>
@@ -6453,14 +6466,14 @@
       </c>
       <c r="C2" s="22"/>
       <c r="D2" s="26" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="22"/>
     </row>
     <row r="3" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B3" s="25" t="n">
         <f aca="false">B2+7</f>
@@ -6473,10 +6486,10 @@
     </row>
     <row r="4" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="22" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C4" s="22"/>
       <c r="D4" s="22"/>
@@ -6497,7 +6510,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
@@ -6505,7 +6518,7 @@
     </row>
     <row r="7" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="22" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B7" s="22" t="n">
         <v>2</v>
@@ -6517,7 +6530,7 @@
     </row>
     <row r="8" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="22" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B8" s="22" t="n">
         <f aca="false">B7-C8</f>
@@ -6533,7 +6546,7 @@
     </row>
     <row r="9" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="22" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B9" s="22" t="n">
         <f aca="false">B8-C9</f>
@@ -6549,7 +6562,7 @@
     </row>
     <row r="10" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="22" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B10" s="22" t="n">
         <f aca="false">B9-C10</f>
@@ -6565,7 +6578,7 @@
     </row>
     <row r="11" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="22" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B11" s="22" t="n">
         <f aca="false">B10-C11</f>
@@ -6581,7 +6594,7 @@
     </row>
     <row r="12" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="22" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B12" s="22" t="n">
         <f aca="false">B11-C12</f>
@@ -6597,15 +6610,14 @@
     </row>
     <row r="13" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="22" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B13" s="22" t="n">
         <f aca="false">B12-C13</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13" s="22" t="n">
-        <f aca="false">COUNTIF(E$17:E$995, "Completed Day 6")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="22"/>
       <c r="E13" s="22"/>
@@ -6613,11 +6625,11 @@
     </row>
     <row r="14" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="22" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B14" s="22" t="n">
         <f aca="false">B13-C14</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C14" s="22" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -6637,16 +6649,16 @@
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="29" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B16" s="29" t="s">
         <v>20</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E16" s="29" t="s">
         <v>25</v>
@@ -6655,683 +6667,689 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B17" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="D17" s="35" t="s">
-        <v>186</v>
-      </c>
-      <c r="E17" s="34"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D17" s="30" t="s">
+        <v>187</v>
+      </c>
+      <c r="E17" s="32" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <v>2</v>
       </c>
       <c r="B18" s="30" t="s">
-        <v>51</v>
-      </c>
-      <c r="D18" s="33"/>
-      <c r="E18" s="34"/>
+        <v>52</v>
+      </c>
+      <c r="D18" s="30" t="s">
+        <v>188</v>
+      </c>
+      <c r="E18" s="32" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <v>3</v>
       </c>
       <c r="B19" s="30"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="34"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="32"/>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
         <v>4</v>
       </c>
       <c r="B20" s="30"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="34"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="32"/>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
         <v>5</v>
       </c>
       <c r="B21" s="30"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="34"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="32"/>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
         <v>6</v>
       </c>
       <c r="B22" s="30"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="34"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="32"/>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
         <v>7</v>
       </c>
       <c r="B23" s="30"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="34"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="32"/>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
         <v>8</v>
       </c>
       <c r="B24" s="30"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="34"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="32"/>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
         <v>9</v>
       </c>
       <c r="B25" s="30"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="34"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="32"/>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
         <v>10</v>
       </c>
       <c r="B26" s="30"/>
-      <c r="D26" s="33"/>
-      <c r="E26" s="34"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="32"/>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
         <v>11</v>
       </c>
       <c r="B27" s="30"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="34"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="32"/>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
         <v>12</v>
       </c>
       <c r="B28" s="30"/>
-      <c r="D28" s="33"/>
-      <c r="E28" s="34"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="32"/>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
         <v>13</v>
       </c>
       <c r="B29" s="30"/>
-      <c r="D29" s="33"/>
-      <c r="E29" s="34"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="32"/>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
         <v>14</v>
       </c>
       <c r="B30" s="30"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="34"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="32"/>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
         <v>15</v>
       </c>
       <c r="B31" s="30"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="34"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="32"/>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
         <v>16</v>
       </c>
       <c r="B32" s="30"/>
-      <c r="D32" s="33"/>
-      <c r="E32" s="34"/>
+      <c r="D32" s="30"/>
+      <c r="E32" s="32"/>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
         <v>17</v>
       </c>
       <c r="B33" s="30"/>
-      <c r="D33" s="33"/>
-      <c r="E33" s="34"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="32"/>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
         <v>18</v>
       </c>
       <c r="B34" s="30"/>
-      <c r="D34" s="33"/>
-      <c r="E34" s="34"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="32"/>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
         <v>19</v>
       </c>
       <c r="B35" s="30"/>
-      <c r="D35" s="33"/>
-      <c r="E35" s="34"/>
+      <c r="D35" s="30"/>
+      <c r="E35" s="32"/>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
         <v>20</v>
       </c>
       <c r="B36" s="30"/>
-      <c r="D36" s="33"/>
-      <c r="E36" s="34"/>
+      <c r="D36" s="30"/>
+      <c r="E36" s="32"/>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
         <v>21</v>
       </c>
       <c r="B37" s="30"/>
-      <c r="D37" s="33"/>
-      <c r="E37" s="34"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="32"/>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
         <v>22</v>
       </c>
       <c r="B38" s="30"/>
-      <c r="D38" s="33"/>
-      <c r="E38" s="34"/>
+      <c r="D38" s="30"/>
+      <c r="E38" s="32"/>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
         <v>23</v>
       </c>
       <c r="B39" s="30"/>
-      <c r="D39" s="33"/>
-      <c r="E39" s="34"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="32"/>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
         <v>24</v>
       </c>
       <c r="B40" s="30"/>
-      <c r="D40" s="33"/>
-      <c r="E40" s="34"/>
+      <c r="D40" s="30"/>
+      <c r="E40" s="32"/>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
         <v>25</v>
       </c>
       <c r="B41" s="30"/>
-      <c r="D41" s="33"/>
-      <c r="E41" s="34"/>
+      <c r="D41" s="30"/>
+      <c r="E41" s="32"/>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
         <v>26</v>
       </c>
       <c r="B42" s="30"/>
-      <c r="D42" s="33"/>
-      <c r="E42" s="34"/>
+      <c r="D42" s="30"/>
+      <c r="E42" s="32"/>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
         <v>27</v>
       </c>
       <c r="B43" s="30"/>
-      <c r="D43" s="33"/>
-      <c r="E43" s="34"/>
+      <c r="D43" s="30"/>
+      <c r="E43" s="32"/>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
         <v>28</v>
       </c>
       <c r="B44" s="30"/>
-      <c r="D44" s="33"/>
-      <c r="E44" s="34"/>
+      <c r="D44" s="30"/>
+      <c r="E44" s="32"/>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="n">
         <v>29</v>
       </c>
       <c r="B45" s="30"/>
-      <c r="D45" s="33"/>
-      <c r="E45" s="34"/>
+      <c r="D45" s="30"/>
+      <c r="E45" s="32"/>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="n">
         <v>30</v>
       </c>
       <c r="B46" s="30"/>
-      <c r="D46" s="33"/>
-      <c r="E46" s="34"/>
+      <c r="D46" s="30"/>
+      <c r="E46" s="32"/>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="n">
         <v>31</v>
       </c>
       <c r="B47" s="30"/>
-      <c r="D47" s="33"/>
-      <c r="E47" s="34"/>
+      <c r="D47" s="30"/>
+      <c r="E47" s="32"/>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="n">
         <v>32</v>
       </c>
       <c r="B48" s="30"/>
-      <c r="D48" s="33"/>
-      <c r="E48" s="34"/>
+      <c r="D48" s="30"/>
+      <c r="E48" s="32"/>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="n">
         <v>33</v>
       </c>
       <c r="B49" s="30"/>
-      <c r="D49" s="33"/>
-      <c r="E49" s="34"/>
+      <c r="D49" s="30"/>
+      <c r="E49" s="32"/>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="n">
         <v>34</v>
       </c>
       <c r="B50" s="30"/>
-      <c r="D50" s="33"/>
-      <c r="E50" s="34"/>
+      <c r="D50" s="30"/>
+      <c r="E50" s="32"/>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="n">
         <v>35</v>
       </c>
       <c r="B51" s="30"/>
-      <c r="D51" s="33"/>
-      <c r="E51" s="34"/>
+      <c r="D51" s="30"/>
+      <c r="E51" s="32"/>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="n">
         <v>36</v>
       </c>
       <c r="B52" s="30"/>
-      <c r="D52" s="33"/>
-      <c r="E52" s="34"/>
+      <c r="D52" s="30"/>
+      <c r="E52" s="32"/>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="n">
         <v>37</v>
       </c>
       <c r="B53" s="30"/>
-      <c r="D53" s="33"/>
-      <c r="E53" s="34"/>
+      <c r="D53" s="30"/>
+      <c r="E53" s="32"/>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="n">
         <v>38</v>
       </c>
       <c r="B54" s="30"/>
-      <c r="D54" s="33"/>
-      <c r="E54" s="34"/>
+      <c r="D54" s="30"/>
+      <c r="E54" s="32"/>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="n">
         <v>39</v>
       </c>
       <c r="B55" s="30"/>
-      <c r="D55" s="33"/>
-      <c r="E55" s="34"/>
+      <c r="D55" s="30"/>
+      <c r="E55" s="32"/>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="n">
         <v>40</v>
       </c>
       <c r="B56" s="30"/>
-      <c r="D56" s="33"/>
-      <c r="E56" s="34"/>
+      <c r="D56" s="30"/>
+      <c r="E56" s="32"/>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="n">
         <v>41</v>
       </c>
       <c r="B57" s="30"/>
-      <c r="D57" s="33"/>
-      <c r="E57" s="34"/>
+      <c r="D57" s="30"/>
+      <c r="E57" s="32"/>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="n">
         <v>42</v>
       </c>
       <c r="B58" s="30"/>
-      <c r="D58" s="33"/>
-      <c r="E58" s="34"/>
+      <c r="D58" s="30"/>
+      <c r="E58" s="32"/>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="n">
         <v>43</v>
       </c>
       <c r="B59" s="30"/>
-      <c r="D59" s="33"/>
-      <c r="E59" s="34"/>
+      <c r="D59" s="30"/>
+      <c r="E59" s="32"/>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="n">
         <v>44</v>
       </c>
       <c r="B60" s="30"/>
-      <c r="D60" s="33"/>
-      <c r="E60" s="34"/>
+      <c r="D60" s="30"/>
+      <c r="E60" s="32"/>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="n">
         <v>45</v>
       </c>
       <c r="B61" s="30"/>
-      <c r="D61" s="33"/>
-      <c r="E61" s="34"/>
+      <c r="D61" s="30"/>
+      <c r="E61" s="32"/>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="n">
         <v>46</v>
       </c>
       <c r="B62" s="30"/>
-      <c r="D62" s="33"/>
-      <c r="E62" s="34"/>
+      <c r="D62" s="30"/>
+      <c r="E62" s="32"/>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="n">
         <v>47</v>
       </c>
       <c r="B63" s="30"/>
-      <c r="D63" s="33"/>
-      <c r="E63" s="34"/>
+      <c r="D63" s="30"/>
+      <c r="E63" s="32"/>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="n">
         <v>48</v>
       </c>
       <c r="B64" s="30"/>
-      <c r="D64" s="33"/>
-      <c r="E64" s="34"/>
+      <c r="D64" s="30"/>
+      <c r="E64" s="32"/>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="n">
         <v>49</v>
       </c>
       <c r="B65" s="30"/>
-      <c r="D65" s="33"/>
-      <c r="E65" s="34"/>
+      <c r="D65" s="30"/>
+      <c r="E65" s="32"/>
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="n">
         <v>50</v>
       </c>
       <c r="B66" s="30"/>
-      <c r="D66" s="33"/>
-      <c r="E66" s="34"/>
+      <c r="D66" s="30"/>
+      <c r="E66" s="32"/>
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="n">
         <v>51</v>
       </c>
       <c r="B67" s="30"/>
-      <c r="D67" s="33"/>
-      <c r="E67" s="34"/>
+      <c r="D67" s="30"/>
+      <c r="E67" s="32"/>
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="n">
         <v>52</v>
       </c>
       <c r="B68" s="30"/>
-      <c r="D68" s="33"/>
-      <c r="E68" s="34"/>
+      <c r="D68" s="30"/>
+      <c r="E68" s="32"/>
     </row>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="n">
         <v>53</v>
       </c>
       <c r="B69" s="30"/>
-      <c r="D69" s="33"/>
-      <c r="E69" s="34"/>
+      <c r="D69" s="30"/>
+      <c r="E69" s="32"/>
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="n">
         <v>54</v>
       </c>
       <c r="B70" s="30"/>
-      <c r="D70" s="33"/>
-      <c r="E70" s="34"/>
+      <c r="D70" s="30"/>
+      <c r="E70" s="32"/>
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="n">
         <v>55</v>
       </c>
       <c r="B71" s="30"/>
-      <c r="D71" s="33"/>
-      <c r="E71" s="34"/>
+      <c r="D71" s="30"/>
+      <c r="E71" s="32"/>
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="n">
         <v>56</v>
       </c>
       <c r="B72" s="30"/>
-      <c r="D72" s="33"/>
-      <c r="E72" s="34"/>
+      <c r="D72" s="30"/>
+      <c r="E72" s="32"/>
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="n">
         <v>57</v>
       </c>
       <c r="B73" s="30"/>
-      <c r="D73" s="33"/>
-      <c r="E73" s="34"/>
+      <c r="D73" s="30"/>
+      <c r="E73" s="32"/>
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="n">
         <v>58</v>
       </c>
       <c r="B74" s="30"/>
-      <c r="D74" s="33"/>
-      <c r="E74" s="34"/>
+      <c r="D74" s="30"/>
+      <c r="E74" s="32"/>
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="n">
         <v>59</v>
       </c>
       <c r="B75" s="30"/>
-      <c r="D75" s="33"/>
-      <c r="E75" s="34"/>
+      <c r="D75" s="30"/>
+      <c r="E75" s="32"/>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="n">
         <v>60</v>
       </c>
       <c r="B76" s="30"/>
-      <c r="D76" s="33"/>
-      <c r="E76" s="34"/>
+      <c r="D76" s="30"/>
+      <c r="E76" s="32"/>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="n">
         <v>61</v>
       </c>
       <c r="B77" s="30"/>
-      <c r="D77" s="33"/>
-      <c r="E77" s="34"/>
+      <c r="D77" s="30"/>
+      <c r="E77" s="32"/>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="n">
         <v>62</v>
       </c>
       <c r="B78" s="30"/>
-      <c r="D78" s="33"/>
-      <c r="E78" s="34"/>
+      <c r="D78" s="30"/>
+      <c r="E78" s="32"/>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="n">
         <v>63</v>
       </c>
       <c r="B79" s="30"/>
-      <c r="D79" s="33"/>
-      <c r="E79" s="34"/>
+      <c r="D79" s="30"/>
+      <c r="E79" s="32"/>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="n">
         <v>64</v>
       </c>
       <c r="B80" s="30"/>
-      <c r="D80" s="33"/>
-      <c r="E80" s="34"/>
+      <c r="D80" s="30"/>
+      <c r="E80" s="32"/>
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="n">
         <v>65</v>
       </c>
       <c r="B81" s="30"/>
-      <c r="D81" s="33"/>
-      <c r="E81" s="34"/>
+      <c r="D81" s="30"/>
+      <c r="E81" s="32"/>
     </row>
     <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="n">
         <v>66</v>
       </c>
       <c r="B82" s="30"/>
-      <c r="D82" s="33"/>
-      <c r="E82" s="34"/>
+      <c r="D82" s="30"/>
+      <c r="E82" s="32"/>
     </row>
     <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="n">
         <v>67</v>
       </c>
       <c r="B83" s="30"/>
-      <c r="D83" s="33"/>
-      <c r="E83" s="34"/>
+      <c r="D83" s="30"/>
+      <c r="E83" s="32"/>
     </row>
     <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="n">
         <v>68</v>
       </c>
       <c r="B84" s="30"/>
-      <c r="D84" s="33"/>
-      <c r="E84" s="34"/>
+      <c r="D84" s="30"/>
+      <c r="E84" s="32"/>
     </row>
     <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="n">
         <v>69</v>
       </c>
       <c r="B85" s="30"/>
-      <c r="D85" s="33"/>
-      <c r="E85" s="34"/>
+      <c r="D85" s="30"/>
+      <c r="E85" s="32"/>
     </row>
     <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="n">
         <v>70</v>
       </c>
       <c r="B86" s="30"/>
-      <c r="D86" s="33"/>
-      <c r="E86" s="34"/>
+      <c r="D86" s="30"/>
+      <c r="E86" s="32"/>
     </row>
     <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="n">
         <v>71</v>
       </c>
       <c r="B87" s="30"/>
-      <c r="D87" s="33"/>
-      <c r="E87" s="34"/>
+      <c r="D87" s="30"/>
+      <c r="E87" s="32"/>
     </row>
     <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="n">
         <v>72</v>
       </c>
       <c r="B88" s="30"/>
-      <c r="D88" s="33"/>
-      <c r="E88" s="34"/>
+      <c r="D88" s="30"/>
+      <c r="E88" s="32"/>
     </row>
     <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="n">
         <v>73</v>
       </c>
       <c r="B89" s="30"/>
-      <c r="D89" s="33"/>
-      <c r="E89" s="34"/>
+      <c r="D89" s="30"/>
+      <c r="E89" s="32"/>
     </row>
     <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="n">
         <v>74</v>
       </c>
       <c r="B90" s="30"/>
-      <c r="D90" s="33"/>
-      <c r="E90" s="34"/>
+      <c r="D90" s="30"/>
+      <c r="E90" s="32"/>
     </row>
     <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="n">
         <v>75</v>
       </c>
       <c r="B91" s="30"/>
-      <c r="D91" s="33"/>
-      <c r="E91" s="34"/>
+      <c r="D91" s="30"/>
+      <c r="E91" s="32"/>
     </row>
     <row r="92" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="n">
         <v>76</v>
       </c>
       <c r="B92" s="30"/>
-      <c r="D92" s="33"/>
-      <c r="E92" s="34"/>
+      <c r="D92" s="30"/>
+      <c r="E92" s="32"/>
     </row>
     <row r="93" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="n">
         <v>77</v>
       </c>
       <c r="B93" s="30"/>
-      <c r="D93" s="33"/>
-      <c r="E93" s="34"/>
+      <c r="D93" s="30"/>
+      <c r="E93" s="32"/>
     </row>
     <row r="94" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="n">
         <v>78</v>
       </c>
       <c r="B94" s="30"/>
-      <c r="D94" s="33"/>
-      <c r="E94" s="34"/>
+      <c r="D94" s="30"/>
+      <c r="E94" s="32"/>
     </row>
     <row r="95" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="n">
         <v>79</v>
       </c>
       <c r="B95" s="30"/>
-      <c r="D95" s="33"/>
-      <c r="E95" s="34"/>
+      <c r="D95" s="30"/>
+      <c r="E95" s="32"/>
     </row>
     <row r="96" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="n">
         <v>80</v>
       </c>
       <c r="B96" s="30"/>
-      <c r="D96" s="33"/>
-      <c r="E96" s="34"/>
+      <c r="D96" s="30"/>
+      <c r="E96" s="32"/>
     </row>
     <row r="97" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="n">
         <v>81</v>
       </c>
       <c r="B97" s="30"/>
-      <c r="D97" s="33"/>
-      <c r="E97" s="34"/>
+      <c r="D97" s="30"/>
+      <c r="E97" s="32"/>
     </row>
     <row r="98" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="n">
         <v>82</v>
       </c>
       <c r="B98" s="30"/>
-      <c r="D98" s="33"/>
-      <c r="E98" s="34"/>
+      <c r="D98" s="30"/>
+      <c r="E98" s="32"/>
     </row>
     <row r="99" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="n">
         <v>83</v>
       </c>
       <c r="B99" s="30"/>
-      <c r="D99" s="33"/>
-      <c r="E99" s="34"/>
+      <c r="D99" s="30"/>
+      <c r="E99" s="32"/>
     </row>
     <row r="100" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="n">
         <v>84</v>
       </c>
       <c r="B100" s="30"/>
-      <c r="D100" s="33"/>
-      <c r="E100" s="34"/>
+      <c r="D100" s="30"/>
+      <c r="E100" s="32"/>
     </row>
   </sheetData>
   <dataValidations count="6">
@@ -7347,7 +7365,7 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" prompt="Select a Feature ID to the left. Then, in this column, list each discrete task needed to implement that feature.&#10;&#10;Example tasks might be &quot;create the Foo class&quot;, &quot;add the Bar method to the (existing) Qux class&quot;, &quot;Find icons for the task bar&quot;, &quot;Update the m" promptTitle="Task Description" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D18:D100" type="none">
+    <dataValidation allowBlank="true" operator="equal" prompt="Select a Feature ID to the left. Then, in this column, list each discrete task needed to implement that feature.&#10;&#10;Example tasks might be &quot;create the Foo class&quot;, &quot;add the Bar method to the (existing) Qux class&quot;, &quot;Find icons for the task bar&quot;, &quot;Update the m" promptTitle="Task Description" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D17:D100" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -7382,7 +7400,7 @@
       <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -7407,7 +7425,7 @@
     </row>
     <row r="2" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B2" s="25" t="n">
         <f aca="false">'Sprint 02 Backlog'!B3</f>
@@ -7415,14 +7433,14 @@
       </c>
       <c r="C2" s="22"/>
       <c r="D2" s="26" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="22"/>
     </row>
     <row r="3" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B3" s="25" t="n">
         <f aca="false">B2+7</f>
@@ -7435,10 +7453,10 @@
     </row>
     <row r="4" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="22" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C4" s="22"/>
       <c r="D4" s="22"/>
@@ -7459,7 +7477,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
@@ -7467,7 +7485,7 @@
     </row>
     <row r="7" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="22" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B7" s="22" t="n">
         <f aca="false">COUNTA(D17:D995)</f>
@@ -7480,7 +7498,7 @@
     </row>
     <row r="8" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="22" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B8" s="22" t="n">
         <f aca="false">B7-C8</f>
@@ -7496,7 +7514,7 @@
     </row>
     <row r="9" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="22" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B9" s="22" t="n">
         <f aca="false">B8-C9</f>
@@ -7512,7 +7530,7 @@
     </row>
     <row r="10" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="22" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B10" s="22" t="n">
         <f aca="false">B9-C10</f>
@@ -7528,7 +7546,7 @@
     </row>
     <row r="11" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="22" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B11" s="22" t="n">
         <f aca="false">B10-C11</f>
@@ -7544,7 +7562,7 @@
     </row>
     <row r="12" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="22" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B12" s="22" t="n">
         <f aca="false">B11-C12</f>
@@ -7560,7 +7578,7 @@
     </row>
     <row r="13" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="22" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B13" s="22" t="n">
         <f aca="false">B12-C13</f>
@@ -7576,7 +7594,7 @@
     </row>
     <row r="14" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="22" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B14" s="22" t="n">
         <f aca="false">B13-C14</f>
@@ -7600,16 +7618,16 @@
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="29" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B16" s="29" t="s">
         <v>20</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E16" s="29" t="s">
         <v>25</v>
@@ -7624,7 +7642,7 @@
       </c>
       <c r="B17" s="33"/>
       <c r="D17" s="35" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="E17" s="34"/>
     </row>
@@ -8341,7 +8359,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -8366,21 +8384,21 @@
     </row>
     <row r="2" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B2" s="25" t="n">
         <v>44873</v>
       </c>
       <c r="C2" s="22"/>
       <c r="D2" s="26" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="22"/>
     </row>
     <row r="3" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B3" s="25" t="n">
         <f aca="false">B2+7</f>
@@ -8393,10 +8411,10 @@
     </row>
     <row r="4" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="22" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C4" s="22"/>
       <c r="D4" s="22"/>
@@ -8417,7 +8435,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
@@ -8425,7 +8443,7 @@
     </row>
     <row r="7" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="22" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B7" s="22" t="n">
         <f aca="false">COUNTA(D17:D995)</f>
@@ -8438,7 +8456,7 @@
     </row>
     <row r="8" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="22" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B8" s="22" t="n">
         <f aca="false">B7-C8</f>
@@ -8454,7 +8472,7 @@
     </row>
     <row r="9" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="22" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B9" s="22" t="n">
         <f aca="false">B8-C9</f>
@@ -8470,7 +8488,7 @@
     </row>
     <row r="10" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="22" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B10" s="22" t="n">
         <f aca="false">B9-C10</f>
@@ -8486,7 +8504,7 @@
     </row>
     <row r="11" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="22" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B11" s="22" t="n">
         <f aca="false">B10-C11</f>
@@ -8502,7 +8520,7 @@
     </row>
     <row r="12" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="22" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B12" s="22" t="n">
         <f aca="false">B11-C12</f>
@@ -8518,7 +8536,7 @@
     </row>
     <row r="13" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="22" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B13" s="22" t="n">
         <f aca="false">B12-C13</f>
@@ -8534,7 +8552,7 @@
     </row>
     <row r="14" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="22" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B14" s="22" t="n">
         <f aca="false">B13-C14</f>
@@ -8558,16 +8576,16 @@
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="29" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B16" s="29" t="s">
         <v>20</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E16" s="29" t="s">
         <v>25</v>
@@ -8582,7 +8600,7 @@
       </c>
       <c r="B17" s="33"/>
       <c r="D17" s="35" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="E17" s="34"/>
     </row>
@@ -9299,7 +9317,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -9324,7 +9342,7 @@
     </row>
     <row r="2" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B2" s="25" t="n">
         <f aca="false">'Sprint 04 Backlog'!B3</f>
@@ -9332,14 +9350,14 @@
       </c>
       <c r="C2" s="22"/>
       <c r="D2" s="26" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="22"/>
     </row>
     <row r="3" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B3" s="25" t="n">
         <f aca="false">B2+7</f>
@@ -9352,10 +9370,10 @@
     </row>
     <row r="4" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="22" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C4" s="22"/>
       <c r="D4" s="22"/>
@@ -9376,7 +9394,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
@@ -9384,7 +9402,7 @@
     </row>
     <row r="7" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="22" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B7" s="22" t="n">
         <f aca="false">COUNTA(D17:D995)</f>
@@ -9397,7 +9415,7 @@
     </row>
     <row r="8" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="22" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B8" s="22" t="n">
         <f aca="false">B7-C8</f>
@@ -9413,7 +9431,7 @@
     </row>
     <row r="9" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="22" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B9" s="22" t="n">
         <f aca="false">B8-C9</f>
@@ -9429,7 +9447,7 @@
     </row>
     <row r="10" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="22" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B10" s="22" t="n">
         <f aca="false">B9-C10</f>
@@ -9445,7 +9463,7 @@
     </row>
     <row r="11" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="22" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B11" s="22" t="n">
         <f aca="false">B10-C11</f>
@@ -9461,7 +9479,7 @@
     </row>
     <row r="12" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="22" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B12" s="22" t="n">
         <f aca="false">B11-C12</f>
@@ -9477,7 +9495,7 @@
     </row>
     <row r="13" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="22" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B13" s="22" t="n">
         <f aca="false">B12-C13</f>
@@ -9493,7 +9511,7 @@
     </row>
     <row r="14" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="22" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B14" s="22" t="n">
         <f aca="false">B13-C14</f>
@@ -9517,16 +9535,16 @@
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="29" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B16" s="29" t="s">
         <v>20</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E16" s="29" t="s">
         <v>25</v>
@@ -9541,7 +9559,7 @@
       </c>
       <c r="B17" s="33"/>
       <c r="D17" s="35" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="E17" s="34"/>
     </row>
@@ -10258,7 +10276,7 @@
       <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -10275,7 +10293,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="D1" s="23" t="s">
         <v>2</v>
@@ -10284,21 +10302,21 @@
     </row>
     <row r="2" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B2" s="25" t="n">
         <v>44894</v>
       </c>
       <c r="C2" s="22"/>
       <c r="D2" s="26" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="22"/>
     </row>
     <row r="3" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B3" s="25" t="n">
         <f aca="false">B2+7</f>
@@ -10311,10 +10329,10 @@
     </row>
     <row r="4" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="22" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C4" s="22"/>
       <c r="D4" s="22"/>
@@ -10335,7 +10353,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
@@ -10343,7 +10361,7 @@
     </row>
     <row r="7" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="22" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B7" s="22" t="n">
         <f aca="false">COUNTA(D17:D995)</f>
@@ -10356,7 +10374,7 @@
     </row>
     <row r="8" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="22" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B8" s="22" t="n">
         <f aca="false">B7-C8</f>
@@ -10372,7 +10390,7 @@
     </row>
     <row r="9" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="22" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B9" s="22" t="n">
         <f aca="false">B8-C9</f>
@@ -10388,7 +10406,7 @@
     </row>
     <row r="10" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="22" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B10" s="22" t="n">
         <f aca="false">B9-C10</f>
@@ -10404,7 +10422,7 @@
     </row>
     <row r="11" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="22" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B11" s="22" t="n">
         <f aca="false">B10-C11</f>
@@ -10420,7 +10438,7 @@
     </row>
     <row r="12" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="22" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B12" s="22" t="n">
         <f aca="false">B11-C12</f>
@@ -10436,7 +10454,7 @@
     </row>
     <row r="13" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="22" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B13" s="22" t="n">
         <f aca="false">B12-C13</f>
@@ -10452,7 +10470,7 @@
     </row>
     <row r="14" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="22" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B14" s="22" t="n">
         <f aca="false">B13-C14</f>
@@ -10471,23 +10489,23 @@
       <c r="B15" s="22"/>
       <c r="C15" s="22"/>
       <c r="D15" s="22" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="E15" s="22"/>
       <c r="F15" s="22"/>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="29" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B16" s="29" t="s">
         <v>20</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E16" s="29" t="s">
         <v>25</v>
@@ -10502,7 +10520,7 @@
       </c>
       <c r="B17" s="33"/>
       <c r="D17" s="35" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="E17" s="34"/>
     </row>

</xml_diff>